<commit_message>
Updated from V2 changes+outputs
Overwrite with code and outputs (including new ablation experiments) as part of post icml revisions
</commit_message>
<xml_diff>
--- a/code/Outputs/annotaters_results/Pasi_gallstone_candidates.xlsx
+++ b/code/Outputs/annotaters_results/Pasi_gallstone_candidates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://medtronicemea-my.sharepoint.com/personal/oferd2_medtronic_com/Documents/Documents/research/InterestingFeats/code/code/Outputs/annotaters_results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{96F56F65-93B1-46BE-AA0E-6F676D9DE0BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{815515F1-7A63-49F8-9D67-CF47C23BAFA6}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="13_ncr:1_{96F56F65-93B1-46BE-AA0E-6F676D9DE0BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B1525BED-1407-E34D-94F0-CD066C72CAB6}"/>
   <bookViews>
-    <workbookView xWindow="435" yWindow="0" windowWidth="33585" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="39260" yWindow="500" windowWidth="37060" windowHeight="21560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -533,6 +533,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -902,22 +903,22 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B34" sqref="B34"/>
+      <selection pane="topRight" activeCell="F44" sqref="F44:I44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="46.42578125" customWidth="1"/>
-    <col min="2" max="2" width="153.7109375" style="5" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" customWidth="1"/>
-    <col min="5" max="5" width="34.28515625" customWidth="1"/>
-    <col min="7" max="7" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="46.5" customWidth="1"/>
+    <col min="2" max="2" width="153.6640625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" customWidth="1"/>
+    <col min="5" max="5" width="34.33203125" customWidth="1"/>
+    <col min="7" max="7" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -946,7 +947,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -975,7 +976,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -1004,7 +1005,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1033,7 +1034,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -1062,7 +1063,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -1091,7 +1092,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -1120,7 +1121,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -1149,7 +1150,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -1178,7 +1179,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -1207,7 +1208,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -1236,7 +1237,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -1265,7 +1266,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -1294,7 +1295,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>36</v>
       </c>
@@ -1323,7 +1324,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>38</v>
       </c>
@@ -1352,7 +1353,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>40</v>
       </c>
@@ -1381,7 +1382,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>42</v>
       </c>
@@ -1410,7 +1411,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>44</v>
       </c>
@@ -1439,7 +1440,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>46</v>
       </c>
@@ -1468,7 +1469,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>48</v>
       </c>
@@ -1497,7 +1498,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>50</v>
       </c>
@@ -1526,7 +1527,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>52</v>
       </c>
@@ -1555,7 +1556,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>54</v>
       </c>
@@ -1584,7 +1585,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>56</v>
       </c>
@@ -1613,7 +1614,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>58</v>
       </c>
@@ -1642,7 +1643,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>60</v>
       </c>
@@ -1671,7 +1672,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>62</v>
       </c>
@@ -1700,7 +1701,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>64</v>
       </c>
@@ -1729,7 +1730,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>66</v>
       </c>
@@ -1758,7 +1759,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>68</v>
       </c>
@@ -1787,7 +1788,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>70</v>
       </c>
@@ -1816,7 +1817,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>72</v>
       </c>
@@ -1845,7 +1846,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>74</v>
       </c>
@@ -1874,7 +1875,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="181.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" ht="181.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>76</v>
       </c>
@@ -1903,7 +1904,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>78</v>
       </c>
@@ -1932,7 +1933,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>80</v>
       </c>
@@ -1961,7 +1962,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>82</v>
       </c>
@@ -1990,7 +1991,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>84</v>
       </c>
@@ -2019,7 +2020,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>86</v>
       </c>
@@ -2048,7 +2049,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>88</v>
       </c>
@@ -2077,7 +2078,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>90</v>
       </c>
@@ -2106,7 +2107,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>92</v>
       </c>
@@ -2135,7 +2136,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>94</v>
       </c>
@@ -2164,7 +2165,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="144" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" ht="144" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>96</v>
       </c>
@@ -2193,7 +2194,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>98</v>
       </c>
@@ -2222,7 +2223,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>101</v>
       </c>
@@ -2239,7 +2240,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="47" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>103</v>
       </c>
@@ -2268,7 +2269,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>105</v>
       </c>
@@ -2297,7 +2298,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>107</v>
       </c>
@@ -2326,7 +2327,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>109</v>
       </c>
@@ -2355,7 +2356,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>111</v>
       </c>
@@ -2384,7 +2385,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>113</v>
       </c>
@@ -2416,9 +2417,9 @@
   </sheetData>
   <autoFilter ref="F1:I52" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <filterColumn colId="3">
-      <filters>
-        <filter val="4"/>
-      </filters>
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
     </filterColumn>
   </autoFilter>
   <dataValidations count="1">
@@ -2427,5 +2428,6 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>